<commit_message>
make an installable  package
</commit_message>
<xml_diff>
--- a/CVX_Kenya/my_graphs/Production Change.xlsx
+++ b/CVX_Kenya/my_graphs/Production Change.xlsx
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-9.29483369551599</v>
+        <v>6.428615036886185</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.0005966205208096653</v>
+        <v>1.179444761626655</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -484,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-2.65279768477194</v>
+        <v>72.19119401741773</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-1.616828121990693</v>
+        <v>0.001212478087836644</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-0.001493057512561791</v>
+        <v>6800.642091352325</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-0.03919737064279616</v>
+        <v>225.860721036559</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>-2.288692418427672</v>
+        <v>12.55734109721379</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>-1.657002884538088</v>
+        <v>0.04257072621840052</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -550,7 +550,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>-0.9812988818157464</v>
+        <v>93.12300139479339</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -561,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>-0.03165692983020563</v>
+        <v>0.6570096939249197</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>-1.451427668333054</v>
+        <v>22.64693908020854</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -580,7 +580,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-0.7710463891271502</v>
+        <v>2.526329814456403</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -591,7 +591,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-74.98937155873864</v>
+        <v>0.01740844821324572</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -602,7 +602,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>-2.419164398917928</v>
+        <v>5440.07830106176</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -613,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>-0.4808939004769854</v>
+        <v>0.0003606278914958239</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>-0.3902365583926439</v>
+        <v>66.62428904755507</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -635,7 +635,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>-0.007818567217327654</v>
+        <v>45.05167570587946</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>-0.4390963484474923</v>
+        <v>2.40918464056449</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -657,7 +657,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>-0.4689986088287696</v>
+        <v>0.01204602731013438</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>-0.03165692983020563</v>
+        <v>0.6570096939249197</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>-1.344290333800018</v>
+        <v>22.16662792675197</v>
       </c>
       <c r="C22">
         <v>0</v>

</xml_diff>